<commit_message>
Add municipal water dedication policies map, issue #3
Also do other cleanup and add information pages for SWSPs and IWSAs, etc.
</commit_message>
<xml_diff>
--- a/workflow/SupportingData/WaterTransfer-CaseStudies/data/transfer-case-studies.xlsx
+++ b/workflow/SupportingData/WaterTransfer-CaseStudies/data/transfer-case-studies.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>URL</t>
   </si>
@@ -72,10 +72,37 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no?</t>
-  </si>
-  <si>
     <t>CaseStudyName</t>
+  </si>
+  <si>
+    <t>Grand Valley Water Users Association Conserved Consumptive Use Pilot Project</t>
+  </si>
+  <si>
+    <t>http://www.grandvalleywaterusers.com/uploads/8/2/6/0/82606774/03-01-17_ccupp_projectdevelopment_final.pdf</t>
+  </si>
+  <si>
+    <t>Mesa</t>
+  </si>
+  <si>
+    <t>Catlin Canal Company Rotational Land Fallowing-Municipal Leasing Pilot Project</t>
+  </si>
+  <si>
+    <t>https://dnrweblink.state.co.us/cwcb/0/edoc/210320/19%2001%2015%202018%20Annual%20Report%20-%20Catlin%20Pilot%20Project%20FINAL.pdf?searchid=3856cf32-c475-4163-840c-5361fa65041f</t>
+  </si>
+  <si>
+    <t>Otero</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Yampa Basin ALternative Agricultural Water Transfer Methods Study</t>
+  </si>
+  <si>
+    <t>https://dnrweblink.state.co.us/cwcb/0/edoc/199193/Yampa%20-%20NC%20Use%20of%20ATM%20to%20Meet%20Non%20%20Consumpt%20Needs_FINALReport%203-28-14_with%20apps.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -131,13 +158,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -462,25 +492,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="1" max="1" width="69.21875" customWidth="1"/>
+    <col min="2" max="2" width="70.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -499,41 +529,104 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6">
+        <v>-103.71323099999999</v>
+      </c>
+      <c r="F2" s="6">
+        <v>38.009126000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6">
+        <v>-108.75243399999999</v>
+      </c>
+      <c r="F3" s="6">
+        <v>39.197431999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E4" s="4">
         <v>-105.10753200000001</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F4" s="4">
         <v>40.286045999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>-107.198581</v>
+      </c>
+      <c r="F6">
+        <v>40.502360000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>